<commit_message>
DATABASE NEK THINGS DONE FOR THE 8 ENTITIES RELATED TO CASH
</commit_message>
<xml_diff>
--- a/DATA_MODELING AND WORKING.xlsx
+++ b/DATA_MODELING AND WORKING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktemi\code\dabo_bet\dabo_bet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA1ADA2-FD20-41FE-8186-44CDD9AF6D67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4691B3C4-2ABC-418C-B442-7AA077C32AB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{194E8500-D8EB-4916-9E2D-0F0C34382F12}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="285">
   <si>
     <t>item_name</t>
   </si>
@@ -255,9 +255,6 @@
     <t>type["yetebelashe", "damaged", "serategna abelashtot"]</t>
   </si>
   <si>
-    <t>product</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -732,9 +729,6 @@
     <t>EXPENSES</t>
   </si>
   <si>
-    <t>for_user - DEFAULT ADMIN</t>
-  </si>
-  <si>
     <t>description - nullable ENA LE PURPOSE NEW</t>
   </si>
   <si>
@@ -768,9 +762,6 @@
     <t>r</t>
   </si>
   <si>
-    <t>DAILY</t>
-  </si>
-  <si>
     <t>COMMISSION</t>
   </si>
   <si>
@@ -786,12 +777,6 @@
     <t>branch_id</t>
   </si>
   <si>
-    <t>discount_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">record_status = [active]/ inactivem lihon ychlal when </t>
-  </si>
-  <si>
     <t>LE REDUNDANCY COPY EVERY SALES DATA HARDCODED ADRGE BECAUSE I DON'T WANT IT TO CHANGE LATER FOR REDUNDANCY PURPOSES</t>
   </si>
   <si>
@@ -870,9 +855,6 @@
     <t>operation</t>
   </si>
   <si>
-    <t>adjustment_type - string legizew until I figure out mninetun</t>
-  </si>
-  <si>
     <t>COMMISSION_ID</t>
   </si>
   <si>
@@ -883,6 +865,21 @@
   </si>
   <si>
     <t>WE NEED TO ADD CATEGORY TO INVENTORY ITEMS TABLE AND SKU AND ALERT QUANTITY TO PRODUCTS OR BRANDS TABLE TO ALLOW US FURTHER ANALYSIS ACCORDING TO ACCOUNTING PRINCIPLES</t>
+  </si>
+  <si>
+    <t>remark - string nullable</t>
+  </si>
+  <si>
+    <t>user_id - DEFAULT ADMIN</t>
+  </si>
+  <si>
+    <t>DAILYSALES</t>
+  </si>
+  <si>
+    <t>discount_amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status = [active]/ inactivem lihon ychlal when </t>
   </si>
 </sst>
 </file>
@@ -1884,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67ECA014-9817-46D2-9F0E-849D0BDD3F91}">
   <dimension ref="A1:AF219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="63" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="63" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1921,7 +1918,7 @@
   <sheetData>
     <row r="1" spans="1:30" s="13" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B1" s="70" t="s">
         <v>50</v>
@@ -2060,11 +2057,11 @@
       </c>
       <c r="J3" s="34">
         <f ca="1">TODAY()</f>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="K3" s="3">
         <f ca="1">TODAY()</f>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -2083,11 +2080,11 @@
       </c>
       <c r="S3" s="3">
         <f ca="1">TODAY()</f>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="T3" s="3">
         <f ca="1">TODAY()</f>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="V3">
         <v>1</v>
@@ -2113,7 +2110,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="73" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B4" s="6">
         <v>2</v>
@@ -2139,11 +2136,11 @@
       </c>
       <c r="J4" s="34">
         <f t="shared" ref="J4:K9" ca="1" si="0">TODAY()</f>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="K4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="M4">
         <v>2</v>
@@ -2162,11 +2159,11 @@
       </c>
       <c r="S4" s="3">
         <f ca="1">TODAY()</f>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="T4" s="3">
         <f ca="1">TODAY()</f>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="V4">
         <v>2</v>
@@ -2192,7 +2189,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="82" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B5" s="6">
         <v>3</v>
@@ -2218,11 +2215,11 @@
       </c>
       <c r="J5" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="K5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="M5">
         <v>3</v>
@@ -2241,11 +2238,11 @@
       </c>
       <c r="S5" s="3">
         <f t="shared" ref="S5:T8" ca="1" si="1">TODAY()</f>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="T5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="V5">
         <v>3</v>
@@ -2271,7 +2268,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="83" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B6" s="6">
         <v>4</v>
@@ -2297,11 +2294,11 @@
       </c>
       <c r="J6" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="K6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="M6">
         <v>4</v>
@@ -2320,11 +2317,11 @@
       </c>
       <c r="S6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="T6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="V6">
         <v>4</v>
@@ -2373,11 +2370,11 @@
       </c>
       <c r="J7" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="K7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="M7">
         <v>5</v>
@@ -2396,11 +2393,11 @@
       </c>
       <c r="S7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="T7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="V7">
         <v>5</v>
@@ -2443,11 +2440,11 @@
       </c>
       <c r="J8" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="M8">
         <v>6</v>
@@ -2466,11 +2463,11 @@
       </c>
       <c r="S8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="T8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="V8">
         <v>6</v>
@@ -2513,11 +2510,11 @@
       </c>
       <c r="J9" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45491</v>
+        <v>45492</v>
       </c>
       <c r="M9">
         <v>7</v>
@@ -2624,7 +2621,7 @@
     </row>
     <row r="11" spans="1:30" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="95" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B11" s="6">
         <v>9</v>
@@ -2819,7 +2816,7 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" s="75" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -2848,7 +2845,7 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" s="75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>37</v>
@@ -2877,7 +2874,7 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" s="76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>1</v>
@@ -2893,7 +2890,7 @@
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M20">
         <v>18</v>
@@ -2901,7 +2898,7 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="76" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2925,7 +2922,7 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="77" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2941,7 +2938,7 @@
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H22" s="40" t="s">
         <v>73</v>
@@ -2953,7 +2950,7 @@
         <v>3</v>
       </c>
       <c r="K22" s="40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M22">
         <v>20</v>
@@ -2961,7 +2958,7 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="77" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -2986,7 +2983,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M23">
         <v>21</v>
@@ -2994,7 +2991,7 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" s="78" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -3019,7 +3016,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M24">
         <v>22</v>
@@ -3027,7 +3024,7 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" s="78" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="41">
@@ -3040,7 +3037,7 @@
         <v>6</v>
       </c>
       <c r="J25" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M25">
         <v>23</v>
@@ -3058,7 +3055,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M26">
         <v>24</v>
@@ -3076,7 +3073,7 @@
         <v>3</v>
       </c>
       <c r="J27" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M27">
         <v>25</v>
@@ -3094,7 +3091,7 @@
         <v>6</v>
       </c>
       <c r="J28" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M28">
         <v>26</v>
@@ -3112,7 +3109,7 @@
         <v>1</v>
       </c>
       <c r="J29" s="41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M29" s="50"/>
       <c r="N29" s="8"/>
@@ -3135,10 +3132,10 @@
         <v>4</v>
       </c>
       <c r="J30" s="41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N30" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
@@ -3153,10 +3150,10 @@
         <v>1</v>
       </c>
       <c r="J31" s="41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N31" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3174,16 +3171,16 @@
         <v>7</v>
       </c>
       <c r="J32" s="41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M32" s="58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N32" s="6"/>
     </row>
     <row r="33" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="41"/>
@@ -3200,7 +3197,7 @@
         <v>69</v>
       </c>
       <c r="P33" s="54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
@@ -3252,13 +3249,13 @@
     <row r="36" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="79"/>
       <c r="B36" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="11"/>
       <c r="F36" s="55" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G36" s="41"/>
       <c r="H36" s="41"/>
@@ -3281,7 +3278,7 @@
     </row>
     <row r="37" spans="1:20" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="79" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>1</v>
@@ -3299,13 +3296,13 @@
         <v>73</v>
       </c>
       <c r="G37" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="H37" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="H37" s="46" t="s">
-        <v>92</v>
-      </c>
       <c r="I37" s="56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J37" s="46"/>
       <c r="M37" s="37"/>
@@ -3335,7 +3332,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I38" s="45"/>
       <c r="J38" s="16"/>
@@ -3360,14 +3357,14 @@
         <v>1</v>
       </c>
       <c r="H39" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="16"/>
     </row>
     <row r="40" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="80" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -3385,7 +3382,7 @@
         <v>4</v>
       </c>
       <c r="H40" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I40" s="45"/>
       <c r="J40" s="16"/>
@@ -3401,7 +3398,7 @@
         <v>4</v>
       </c>
       <c r="H41" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I41" s="45"/>
       <c r="J41" s="44"/>
@@ -3432,7 +3429,7 @@
         <v>73</v>
       </c>
       <c r="P42" s="51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
@@ -3445,7 +3442,7 @@
         <v>1</v>
       </c>
       <c r="N43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O43">
         <v>1</v>
@@ -3456,7 +3453,7 @@
     </row>
     <row r="44" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="81" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -3471,7 +3468,7 @@
         <v>2</v>
       </c>
       <c r="N44" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O44">
         <v>2</v>
@@ -3483,7 +3480,7 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="81" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>66</v>
@@ -3495,7 +3492,7 @@
         <v>3</v>
       </c>
       <c r="N45" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O45">
         <v>3</v>
@@ -3507,13 +3504,13 @@
     </row>
     <row r="46" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="81" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D46" t="s">
         <v>74</v>
@@ -3522,16 +3519,16 @@
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M46" s="6">
         <v>4</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O46">
         <v>4</v>
@@ -3553,7 +3550,7 @@
         <v>5</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O47">
         <v>5</v>
@@ -3564,7 +3561,7 @@
     </row>
     <row r="48" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="81" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="F48" s="5"/>
       <c r="K48" s="6"/>
@@ -3572,7 +3569,7 @@
         <v>6</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O48">
         <v>6</v>
@@ -3588,7 +3585,7 @@
         <v>7</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O49">
         <v>1</v>
@@ -3596,13 +3593,13 @@
     </row>
     <row r="50" spans="1:32" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="89" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F50" s="5"/>
       <c r="K50" s="6"/>
       <c r="L50" s="66"/>
       <c r="M50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="1:32" x14ac:dyDescent="0.3">
@@ -3626,19 +3623,19 @@
     </row>
     <row r="55" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="90" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C55" s="39"/>
       <c r="D55" s="63"/>
       <c r="E55" s="92" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F55" s="52"/>
       <c r="G55" s="52"/>
       <c r="H55" s="52"/>
       <c r="I55" s="52"/>
       <c r="J55" s="92" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K55" s="52"/>
       <c r="L55" s="52"/>
@@ -3653,7 +3650,7 @@
         <v>22</v>
       </c>
       <c r="D56" s="59" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E56" s="91" t="s">
         <v>1</v>
@@ -3662,13 +3659,13 @@
         <v>75</v>
       </c>
       <c r="G56" s="91" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="H56" s="91" t="s">
         <v>3</v>
       </c>
       <c r="I56" s="91" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="J56" s="91" t="s">
         <v>1</v>
@@ -3677,13 +3674,13 @@
         <v>64</v>
       </c>
       <c r="L56" s="91" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="M56" s="91" t="s">
         <v>3</v>
       </c>
       <c r="N56" s="91" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="57" spans="1:32" x14ac:dyDescent="0.3">
@@ -3691,10 +3688,10 @@
         <v>1</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D57" s="64" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E57" s="6"/>
       <c r="J57" s="5"/>
@@ -3706,10 +3703,10 @@
         <v>2</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D58" s="64" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="E58"/>
       <c r="F58" s="6"/>
@@ -3722,10 +3719,10 @@
         <v>3</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D59" s="64" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -3769,7 +3766,7 @@
     </row>
     <row r="63" spans="1:32" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A63" s="93" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -3796,7 +3793,7 @@
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B64" s="60" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C64" s="60" t="s">
         <v>71</v>
@@ -3806,10 +3803,10 @@
       <c r="F64" s="60"/>
       <c r="G64" s="61"/>
       <c r="H64" s="13" t="s">
-        <v>247</v>
+        <v>282</v>
       </c>
       <c r="I64" s="88" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="L64" s="6"/>
       <c r="N64" s="6"/>
@@ -3825,43 +3822,43 @@
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B65" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="C65" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="D65" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="E65" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="F65" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="G65" s="87" t="s">
+        <v>256</v>
+      </c>
+      <c r="H65" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="I65" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="J65" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="C65" s="59" t="s">
-        <v>236</v>
-      </c>
-      <c r="D65" s="59" t="s">
-        <v>233</v>
-      </c>
-      <c r="E65" s="59" t="s">
+      <c r="K65" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="F65" s="59" t="s">
-        <v>242</v>
-      </c>
-      <c r="G65" s="87" t="s">
-        <v>261</v>
-      </c>
-      <c r="H65" s="62" t="s">
-        <v>238</v>
-      </c>
-      <c r="I65" s="62" t="s">
-        <v>239</v>
-      </c>
-      <c r="J65" s="62" t="s">
+      <c r="L65" s="62" t="s">
         <v>240</v>
       </c>
-      <c r="K65" s="62" t="s">
-        <v>237</v>
-      </c>
-      <c r="L65" s="62" t="s">
-        <v>242</v>
-      </c>
       <c r="M65" s="62" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="N65" s="62" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="U65"/>
       <c r="W65" s="1"/>
@@ -3875,7 +3872,7 @@
     </row>
     <row r="66" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" s="84" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E66"/>
       <c r="F66" s="4"/>
@@ -3940,7 +3937,7 @@
     </row>
     <row r="68" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="84" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E68"/>
       <c r="F68" s="4"/>
@@ -3974,7 +3971,7 @@
     </row>
     <row r="69" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="84" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E69"/>
       <c r="F69" s="4"/>
@@ -4039,7 +4036,7 @@
     </row>
     <row r="71" spans="1:32" ht="72" x14ac:dyDescent="0.3">
       <c r="A71" s="95" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E71"/>
       <c r="F71" s="4"/>
@@ -4095,13 +4092,13 @@
     <row r="74" spans="1:32" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="73"/>
       <c r="B74" s="13" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D74" s="86"/>
       <c r="E74" s="86"/>
       <c r="G74" s="67"/>
       <c r="H74" s="15" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="I74" s="69"/>
       <c r="J74" s="69"/>
@@ -4113,24 +4110,24 @@
       <c r="AB74" s="15"/>
       <c r="AD74" s="14"/>
     </row>
-    <row r="75" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A75" s="74" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B75" s="59" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C75" s="59" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="D75" s="59" t="s">
-        <v>239</v>
+        <v>283</v>
       </c>
       <c r="E75" s="59" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F75" s="59" t="s">
-        <v>254</v>
+        <v>284</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" s="59" t="s">
@@ -4140,7 +4137,7 @@
         <v>22</v>
       </c>
       <c r="J75" s="59" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K75" s="59"/>
       <c r="L75" s="59"/>
@@ -4155,7 +4152,7 @@
         <v>1</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
@@ -4163,7 +4160,7 @@
     </row>
     <row r="77" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="74" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B77" s="13">
         <v>2</v>
@@ -4180,7 +4177,7 @@
     </row>
     <row r="78" spans="1:32" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A78" s="79" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B78" s="13">
         <v>3</v>
@@ -4223,7 +4220,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="74" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B81" s="13">
         <v>6</v>
@@ -4238,7 +4235,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="74" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B82" s="13">
         <v>7</v>
@@ -4251,7 +4248,7 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="74" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="1"/>
@@ -4260,7 +4257,7 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="74" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="1"/>
@@ -4269,7 +4266,7 @@
     </row>
     <row r="85" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A85" s="74" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F85" s="6"/>
       <c r="G85" s="1"/>
@@ -4278,10 +4275,10 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="74" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C86" s="13"/>
       <c r="F86" s="6"/>
@@ -4291,22 +4288,22 @@
     </row>
     <row r="87" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A87" s="74" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B87" s="59" t="s">
         <v>1</v>
       </c>
       <c r="C87" s="59" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D87" s="59" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E87" s="59"/>
       <c r="F87" s="59"/>
       <c r="G87" s="1"/>
       <c r="H87" s="15" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="L87" s="6"/>
     </row>
@@ -4402,7 +4399,7 @@
     </row>
     <row r="98" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B98" s="48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
@@ -4427,13 +4424,13 @@
     </row>
     <row r="100" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B100" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C100" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="C100" s="40" t="s">
+      <c r="D100" s="40" t="s">
         <v>97</v>
-      </c>
-      <c r="D100" s="40" t="s">
-        <v>98</v>
       </c>
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
@@ -4447,13 +4444,13 @@
     </row>
     <row r="101" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B101" s="41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C101" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D101" s="41" t="s">
         <v>99</v>
-      </c>
-      <c r="D101" s="41" t="s">
-        <v>100</v>
       </c>
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
@@ -4467,13 +4464,13 @@
     </row>
     <row r="102" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B102" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C102" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="C102" s="41" t="s">
+      <c r="D102" s="41" t="s">
         <v>102</v>
-      </c>
-      <c r="D102" s="41" t="s">
-        <v>103</v>
       </c>
       <c r="F102" s="6"/>
       <c r="G102" s="6"/>
@@ -4490,10 +4487,10 @@
         <v>27</v>
       </c>
       <c r="C103" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D103" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F103" s="6"/>
       <c r="G103" s="6"/>
@@ -4510,10 +4507,10 @@
         <v>2</v>
       </c>
       <c r="C104" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D104" s="41" t="s">
         <v>105</v>
-      </c>
-      <c r="D104" s="41" t="s">
-        <v>106</v>
       </c>
       <c r="F104" s="6"/>
       <c r="G104" s="6"/>
@@ -4527,13 +4524,13 @@
     </row>
     <row r="105" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B105" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C105" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="C105" s="41" t="s">
+      <c r="D105" s="41" t="s">
         <v>108</v>
-      </c>
-      <c r="D105" s="41" t="s">
-        <v>109</v>
       </c>
       <c r="F105" s="6"/>
       <c r="G105" s="6"/>
@@ -4547,13 +4544,13 @@
     </row>
     <row r="106" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B106" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C106" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C106" s="41" t="s">
+      <c r="D106" s="41" t="s">
         <v>111</v>
-      </c>
-      <c r="D106" s="41" t="s">
-        <v>112</v>
       </c>
       <c r="F106" s="6"/>
       <c r="G106" s="6"/>
@@ -4567,13 +4564,13 @@
     </row>
     <row r="107" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B107" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C107" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D107" s="41" t="s">
         <v>113</v>
-      </c>
-      <c r="C107" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="D107" s="41" t="s">
-        <v>114</v>
       </c>
       <c r="F107" s="6"/>
       <c r="G107" s="6"/>
@@ -4587,13 +4584,13 @@
     </row>
     <row r="108" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B108" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C108" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="C108" s="41" t="s">
+      <c r="D108" s="41" t="s">
         <v>116</v>
-      </c>
-      <c r="D108" s="41" t="s">
-        <v>117</v>
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
@@ -4618,7 +4615,7 @@
     </row>
     <row r="110" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B110" s="48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F110" s="6"/>
       <c r="G110" s="6"/>
@@ -4643,13 +4640,13 @@
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B112" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C112" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="C112" s="40" t="s">
+      <c r="D112" s="40" t="s">
         <v>97</v>
-      </c>
-      <c r="D112" s="40" t="s">
-        <v>98</v>
       </c>
       <c r="F112" s="6"/>
       <c r="G112" s="6"/>
@@ -4666,10 +4663,10 @@
         <v>64</v>
       </c>
       <c r="C113" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D113" s="41" t="s">
         <v>99</v>
-      </c>
-      <c r="D113" s="41" t="s">
-        <v>100</v>
       </c>
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
@@ -4686,10 +4683,10 @@
         <v>0</v>
       </c>
       <c r="C114" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D114" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F114" s="6"/>
       <c r="G114" s="6"/>
@@ -4703,13 +4700,13 @@
     </row>
     <row r="115" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B115" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C115" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D115" s="41" t="s">
         <v>120</v>
-      </c>
-      <c r="C115" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D115" s="41" t="s">
-        <v>121</v>
       </c>
       <c r="F115" s="6"/>
       <c r="G115" s="6"/>
@@ -4723,13 +4720,13 @@
     </row>
     <row r="116" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B116" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C116" s="41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D116" s="41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F116" s="6"/>
       <c r="G116" s="6"/>
@@ -4743,13 +4740,13 @@
     </row>
     <row r="117" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B117" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C117" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D117" s="41" t="s">
         <v>123</v>
-      </c>
-      <c r="C117" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="D117" s="41" t="s">
-        <v>124</v>
       </c>
       <c r="F117" s="6"/>
       <c r="G117" s="6"/>
@@ -4763,13 +4760,13 @@
     </row>
     <row r="118" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B118" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="C118" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D118" s="41" t="s">
         <v>125</v>
-      </c>
-      <c r="C118" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="D118" s="41" t="s">
-        <v>126</v>
       </c>
       <c r="F118" s="6"/>
       <c r="G118" s="6"/>
@@ -4783,13 +4780,13 @@
     </row>
     <row r="119" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B119" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="C119" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D119" s="41" t="s">
         <v>127</v>
-      </c>
-      <c r="C119" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="D119" s="41" t="s">
-        <v>128</v>
       </c>
       <c r="F119" s="6"/>
       <c r="G119" s="6"/>
@@ -4803,13 +4800,13 @@
     </row>
     <row r="120" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B120" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C120" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D120" s="41" t="s">
         <v>129</v>
-      </c>
-      <c r="C120" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="D120" s="41" t="s">
-        <v>130</v>
       </c>
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
@@ -4823,13 +4820,13 @@
     </row>
     <row r="121" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B121" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C121" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C121" s="41" t="s">
-        <v>111</v>
-      </c>
       <c r="D121" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F121" s="6"/>
       <c r="G121" s="6"/>
@@ -4843,13 +4840,13 @@
     </row>
     <row r="122" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B122" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C122" s="41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D122" s="41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F122" s="6"/>
       <c r="G122" s="6"/>
@@ -4874,7 +4871,7 @@
     </row>
     <row r="124" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B124" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F124" s="6"/>
       <c r="G124" s="6"/>
@@ -4899,13 +4896,13 @@
     </row>
     <row r="126" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B126" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C126" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="C126" s="40" t="s">
+      <c r="D126" s="40" t="s">
         <v>97</v>
-      </c>
-      <c r="D126" s="40" t="s">
-        <v>98</v>
       </c>
       <c r="F126" s="6"/>
       <c r="G126" s="6"/>
@@ -4922,10 +4919,10 @@
         <v>73</v>
       </c>
       <c r="C127" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D127" s="41" t="s">
         <v>99</v>
-      </c>
-      <c r="D127" s="41" t="s">
-        <v>100</v>
       </c>
       <c r="F127" s="6"/>
       <c r="G127" s="6"/>
@@ -4939,13 +4936,13 @@
     </row>
     <row r="128" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B128" s="41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C128" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D128" s="41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F128" s="6"/>
       <c r="G128" s="6"/>
@@ -4959,13 +4956,13 @@
     </row>
     <row r="129" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B129" s="41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C129" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D129" s="41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F129" s="6"/>
       <c r="G129" s="6"/>
@@ -4979,13 +4976,13 @@
     </row>
     <row r="130" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B130" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C130" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D130" s="41" t="s">
         <v>136</v>
-      </c>
-      <c r="C130" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="D130" s="41" t="s">
-        <v>137</v>
       </c>
       <c r="F130" s="6"/>
       <c r="G130" s="6"/>
@@ -4999,13 +4996,13 @@
     </row>
     <row r="131" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B131" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C131" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D131" s="41" t="s">
         <v>138</v>
-      </c>
-      <c r="C131" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="D131" s="41" t="s">
-        <v>139</v>
       </c>
       <c r="F131" s="6"/>
       <c r="G131" s="6"/>
@@ -5019,13 +5016,13 @@
     </row>
     <row r="132" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B132" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C132" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C132" s="41" t="s">
-        <v>111</v>
-      </c>
       <c r="D132" s="41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F132" s="6"/>
       <c r="G132" s="6"/>
@@ -5039,13 +5036,13 @@
     </row>
     <row r="133" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B133" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C133" s="41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D133" s="41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F133" s="6"/>
       <c r="G133" s="6"/>
@@ -5070,7 +5067,7 @@
     </row>
     <row r="135" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B135" s="48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F135" s="6"/>
       <c r="G135" s="6"/>
@@ -5095,13 +5092,13 @@
     </row>
     <row r="137" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B137" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C137" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="C137" s="40" t="s">
+      <c r="D137" s="40" t="s">
         <v>97</v>
-      </c>
-      <c r="D137" s="40" t="s">
-        <v>98</v>
       </c>
       <c r="F137" s="6"/>
       <c r="G137" s="6"/>
@@ -5115,13 +5112,13 @@
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B138" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C138" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D138" s="41" t="s">
         <v>99</v>
-      </c>
-      <c r="D138" s="41" t="s">
-        <v>100</v>
       </c>
       <c r="F138" s="6"/>
       <c r="G138" s="6"/>
@@ -5138,10 +5135,10 @@
         <v>73</v>
       </c>
       <c r="C139" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D139" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F139" s="6"/>
       <c r="G139" s="6"/>
@@ -5158,10 +5155,10 @@
         <v>64</v>
       </c>
       <c r="C140" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D140" s="41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F140" s="6"/>
       <c r="G140" s="6"/>
@@ -5178,10 +5175,10 @@
         <v>3</v>
       </c>
       <c r="C141" s="41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D141" s="41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F141" s="6"/>
       <c r="G141" s="6"/>
@@ -5195,13 +5192,13 @@
     </row>
     <row r="142" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B142" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C142" s="41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D142" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F142" s="6"/>
       <c r="G142" s="6"/>
@@ -5215,13 +5212,13 @@
     </row>
     <row r="143" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B143" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C143" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C143" s="41" t="s">
-        <v>111</v>
-      </c>
       <c r="D143" s="41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F143" s="6"/>
       <c r="G143" s="6"/>
@@ -5235,13 +5232,13 @@
     </row>
     <row r="144" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B144" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C144" s="41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D144" s="41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F144" s="6"/>
       <c r="G144" s="6"/>
@@ -5266,7 +5263,7 @@
     </row>
     <row r="146" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B146" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F146" s="6"/>
       <c r="G146" s="6"/>
@@ -5291,13 +5288,13 @@
     </row>
     <row r="148" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B148" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C148" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="C148" s="40" t="s">
+      <c r="D148" s="40" t="s">
         <v>97</v>
-      </c>
-      <c r="D148" s="40" t="s">
-        <v>98</v>
       </c>
       <c r="F148" s="6"/>
       <c r="G148" s="6"/>
@@ -5311,13 +5308,13 @@
     </row>
     <row r="149" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B149" s="41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C149" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D149" s="41" t="s">
         <v>99</v>
-      </c>
-      <c r="D149" s="41" t="s">
-        <v>100</v>
       </c>
       <c r="F149" s="6"/>
       <c r="G149" s="6"/>
@@ -5331,13 +5328,13 @@
     </row>
     <row r="150" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B150" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="C150" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D150" s="41" t="s">
         <v>149</v>
-      </c>
-      <c r="C150" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D150" s="41" t="s">
-        <v>150</v>
       </c>
       <c r="F150" s="6"/>
       <c r="G150" s="6"/>
@@ -5351,13 +5348,13 @@
     </row>
     <row r="151" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B151" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="C151" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D151" s="41" t="s">
         <v>151</v>
-      </c>
-      <c r="C151" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D151" s="41" t="s">
-        <v>152</v>
       </c>
       <c r="F151" s="6"/>
       <c r="G151" s="6"/>
@@ -5371,13 +5368,13 @@
     </row>
     <row r="152" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B152" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="C152" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="C152" s="41" t="s">
+      <c r="D152" s="41" t="s">
         <v>154</v>
-      </c>
-      <c r="D152" s="41" t="s">
-        <v>155</v>
       </c>
       <c r="F152" s="6"/>
       <c r="G152" s="6"/>
@@ -5391,13 +5388,13 @@
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B153" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C153" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D153" s="41" t="s">
         <v>156</v>
-      </c>
-      <c r="C153" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D153" s="41" t="s">
-        <v>157</v>
       </c>
       <c r="F153" s="6"/>
       <c r="G153" s="6"/>
@@ -5411,13 +5408,13 @@
     </row>
     <row r="154" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B154" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="C154" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D154" s="41" t="s">
         <v>158</v>
-      </c>
-      <c r="C154" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="D154" s="41" t="s">
-        <v>159</v>
       </c>
       <c r="F154" s="6"/>
       <c r="G154" s="6"/>
@@ -5431,13 +5428,13 @@
     </row>
     <row r="155" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B155" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C155" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C155" s="41" t="s">
-        <v>111</v>
-      </c>
       <c r="D155" s="41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F155" s="6"/>
       <c r="G155" s="6"/>
@@ -5451,13 +5448,13 @@
     </row>
     <row r="156" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B156" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C156" s="41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D156" s="41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F156" s="6"/>
       <c r="G156" s="6"/>
@@ -5482,7 +5479,7 @@
     </row>
     <row r="158" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B158" s="48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F158" s="6"/>
       <c r="G158" s="6"/>
@@ -5508,7 +5505,7 @@
     </row>
     <row r="160" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B160" s="49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F160" s="6"/>
       <c r="G160" s="6"/>
@@ -5522,7 +5519,7 @@
     </row>
     <row r="161" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B161" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F161" s="6"/>
       <c r="G161" s="6"/>
@@ -5536,7 +5533,7 @@
     </row>
     <row r="162" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B162" s="49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F162" s="6"/>
       <c r="G162" s="6"/>
@@ -5550,7 +5547,7 @@
     </row>
     <row r="163" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B163" s="49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F163" s="6"/>
       <c r="G163" s="6"/>
@@ -5564,7 +5561,7 @@
     </row>
     <row r="164" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B164" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F164" s="6"/>
       <c r="G164" s="6"/>
@@ -5578,7 +5575,7 @@
     </row>
     <row r="165" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B165" s="49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F165" s="6"/>
       <c r="G165" s="6"/>
@@ -5592,7 +5589,7 @@
     </row>
     <row r="166" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B166" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F166" s="6"/>
       <c r="G166" s="6"/>
@@ -5606,7 +5603,7 @@
     </row>
     <row r="167" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B167" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F167" s="6"/>
       <c r="G167" s="6"/>
@@ -5620,7 +5617,7 @@
     </row>
     <row r="168" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B168" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F168" s="6"/>
       <c r="G168" s="6"/>
@@ -5634,7 +5631,7 @@
     </row>
     <row r="169" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B169" s="49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F169" s="6"/>
       <c r="G169" s="6"/>
@@ -5648,7 +5645,7 @@
     </row>
     <row r="170" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B170" s="49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F170" s="6"/>
       <c r="G170" s="6"/>
@@ -5662,7 +5659,7 @@
     </row>
     <row r="171" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B171" s="49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F171" s="6"/>
       <c r="G171" s="6"/>
@@ -5688,7 +5685,7 @@
     </row>
     <row r="173" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B173" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F173" s="6"/>
       <c r="G173" s="6"/>
@@ -5702,7 +5699,7 @@
     </row>
     <row r="174" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B174" s="49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F174" s="6"/>
       <c r="G174" s="6"/>
@@ -5716,7 +5713,7 @@
     </row>
     <row r="175" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B175" s="49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F175" s="6"/>
       <c r="G175" s="6"/>
@@ -5730,7 +5727,7 @@
     </row>
     <row r="176" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B176" s="49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F176" s="6"/>
       <c r="G176" s="6"/>
@@ -5744,7 +5741,7 @@
     </row>
     <row r="177" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B177" s="49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F177" s="6"/>
       <c r="G177" s="6"/>
@@ -5758,7 +5755,7 @@
     </row>
     <row r="178" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B178" s="49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F178" s="6"/>
       <c r="G178" s="6"/>
@@ -5772,7 +5769,7 @@
     </row>
     <row r="179" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B179" s="49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F179" s="6"/>
       <c r="G179" s="6"/>
@@ -5786,7 +5783,7 @@
     </row>
     <row r="180" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B180" s="49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F180" s="6"/>
       <c r="G180" s="6"/>
@@ -5800,7 +5797,7 @@
     </row>
     <row r="181" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B181" s="49" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F181" s="6"/>
       <c r="G181" s="6"/>
@@ -5814,7 +5811,7 @@
     </row>
     <row r="182" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B182" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F182" s="6"/>
       <c r="G182" s="6"/>
@@ -5828,7 +5825,7 @@
     </row>
     <row r="183" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B183" s="49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F183" s="6"/>
       <c r="G183" s="6"/>
@@ -5842,7 +5839,7 @@
     </row>
     <row r="184" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B184" s="49" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F184" s="6"/>
       <c r="G184" s="6"/>
@@ -5856,7 +5853,7 @@
     </row>
     <row r="185" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B185" s="49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F185" s="6"/>
       <c r="G185" s="6"/>
@@ -5882,7 +5879,7 @@
     </row>
     <row r="187" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B187" s="49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F187" s="6"/>
       <c r="G187" s="6"/>
@@ -5896,7 +5893,7 @@
     </row>
     <row r="188" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B188" s="49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F188" s="6"/>
       <c r="G188" s="6"/>
@@ -5910,7 +5907,7 @@
     </row>
     <row r="189" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B189" s="49" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F189" s="6"/>
       <c r="G189" s="6"/>
@@ -5924,7 +5921,7 @@
     </row>
     <row r="190" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B190" s="49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F190" s="6"/>
       <c r="G190" s="6"/>
@@ -5938,7 +5935,7 @@
     </row>
     <row r="191" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B191" s="49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F191" s="6"/>
       <c r="G191" s="6"/>
@@ -5952,7 +5949,7 @@
     </row>
     <row r="192" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B192" s="49" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F192" s="6"/>
       <c r="G192" s="6"/>
@@ -5966,7 +5963,7 @@
     </row>
     <row r="193" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B193" s="49" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F193" s="6"/>
       <c r="G193" s="6"/>
@@ -5980,7 +5977,7 @@
     </row>
     <row r="194" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B194" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F194" s="6"/>
       <c r="G194" s="6"/>
@@ -5994,7 +5991,7 @@
     </row>
     <row r="195" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B195" s="49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F195" s="6"/>
       <c r="G195" s="6"/>
@@ -6008,7 +6005,7 @@
     </row>
     <row r="196" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B196" s="49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F196" s="6"/>
       <c r="G196" s="6"/>
@@ -6034,7 +6031,7 @@
     </row>
     <row r="198" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B198" s="49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F198" s="6"/>
       <c r="G198" s="6"/>
@@ -6048,7 +6045,7 @@
     </row>
     <row r="199" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B199" s="49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F199" s="6"/>
       <c r="G199" s="6"/>
@@ -6062,7 +6059,7 @@
     </row>
     <row r="200" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B200" s="49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F200" s="6"/>
       <c r="G200" s="6"/>
@@ -6076,7 +6073,7 @@
     </row>
     <row r="201" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B201" s="49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F201" s="6"/>
       <c r="G201" s="6"/>
@@ -6090,7 +6087,7 @@
     </row>
     <row r="202" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B202" s="49" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F202" s="6"/>
       <c r="G202" s="6"/>
@@ -6104,27 +6101,27 @@
     </row>
     <row r="203" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B203" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="204" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B204" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="205" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B205" s="49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="206" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B206" s="49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="207" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B207" s="49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="208" spans="2:14" x14ac:dyDescent="0.3">
@@ -6132,57 +6129,57 @@
     </row>
     <row r="209" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B209" s="49" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="210" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B210" s="49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="211" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B211" s="49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="212" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B212" s="49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="213" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B213" s="49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="214" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B214" s="49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="215" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B215" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="216" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B216" s="49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="217" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B217" s="49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="218" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B218" s="49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="219" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B219" s="49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BEFORE PURGIN EEVRY CSS AND JS FILE AND AFTER EVERY POSSIBLE CRUD FOR MY ENTITIES
</commit_message>
<xml_diff>
--- a/DATA_MODELING AND WORKING.xlsx
+++ b/DATA_MODELING AND WORKING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktemi\code\dabo_bet\dabo_bet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4691B3C4-2ABC-418C-B442-7AA077C32AB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AB8D67-924D-4F62-B7AC-5C05B47D160F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{194E8500-D8EB-4916-9E2D-0F0C34382F12}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="286">
   <si>
     <t>item_name</t>
   </si>
@@ -252,9 +252,6 @@
     <t>for date</t>
   </si>
   <si>
-    <t>type["yetebelashe", "damaged", "serategna abelashtot"]</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -880,6 +877,12 @@
   </si>
   <si>
     <t xml:space="preserve">status = [active]/ inactivem lihon ychlal when </t>
+  </si>
+  <si>
+    <t>type["stale", "damaged", "worker_error"]</t>
+  </si>
+  <si>
+    <t>remark</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1020,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1402,10 +1405,49 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1417,7 +1459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1560,10 +1602,18 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1881,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67ECA014-9817-46D2-9F0E-849D0BDD3F91}">
   <dimension ref="A1:AF219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="63" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="G49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P56" sqref="P56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1891,7 +1941,7 @@
     <col min="2" max="2" width="26.33203125" customWidth="1"/>
     <col min="3" max="3" width="25.88671875" customWidth="1"/>
     <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="33.44140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="34.6640625" customWidth="1"/>
     <col min="7" max="7" width="31.88671875" customWidth="1"/>
     <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
@@ -1918,7 +1968,7 @@
   <sheetData>
     <row r="1" spans="1:30" s="13" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="70" t="s">
         <v>50</v>
@@ -2110,7 +2160,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="73" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B4" s="6">
         <v>2</v>
@@ -2189,7 +2239,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="82" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5" s="6">
         <v>3</v>
@@ -2268,7 +2318,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="83" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B6" s="6">
         <v>4</v>
@@ -2620,8 +2670,8 @@
       </c>
     </row>
     <row r="11" spans="1:30" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="95" t="s">
-        <v>279</v>
+      <c r="A11" s="94" t="s">
+        <v>278</v>
       </c>
       <c r="B11" s="6">
         <v>9</v>
@@ -2816,7 +2866,7 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" s="75" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -2845,7 +2895,7 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" s="75" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>37</v>
@@ -2874,7 +2924,7 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" s="76" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>1</v>
@@ -2890,7 +2940,7 @@
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M20">
         <v>18</v>
@@ -2898,7 +2948,7 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2922,7 +2972,7 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2938,7 +2988,7 @@
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H22" s="40" t="s">
         <v>73</v>
@@ -2950,7 +3000,7 @@
         <v>3</v>
       </c>
       <c r="K22" s="40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M22">
         <v>20</v>
@@ -2958,7 +3008,7 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="77" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -2983,7 +3033,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M23">
         <v>21</v>
@@ -2991,7 +3041,7 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" s="78" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -3016,7 +3066,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M24">
         <v>22</v>
@@ -3024,7 +3074,7 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" s="78" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="41">
@@ -3037,7 +3087,7 @@
         <v>6</v>
       </c>
       <c r="J25" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M25">
         <v>23</v>
@@ -3055,7 +3105,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M26">
         <v>24</v>
@@ -3073,7 +3123,7 @@
         <v>3</v>
       </c>
       <c r="J27" s="41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M27">
         <v>25</v>
@@ -3091,7 +3141,7 @@
         <v>6</v>
       </c>
       <c r="J28" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M28">
         <v>26</v>
@@ -3109,7 +3159,7 @@
         <v>1</v>
       </c>
       <c r="J29" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M29" s="50"/>
       <c r="N29" s="8"/>
@@ -3132,10 +3182,10 @@
         <v>4</v>
       </c>
       <c r="J30" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N30" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
@@ -3150,10 +3200,10 @@
         <v>1</v>
       </c>
       <c r="J31" s="41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3171,16 +3221,16 @@
         <v>7</v>
       </c>
       <c r="J32" s="41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M32" s="58" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N32" s="6"/>
     </row>
     <row r="33" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="57" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="41"/>
@@ -3197,7 +3247,7 @@
         <v>69</v>
       </c>
       <c r="P33" s="54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
@@ -3249,13 +3299,13 @@
     <row r="36" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="79"/>
       <c r="B36" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="11"/>
       <c r="F36" s="55" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G36" s="41"/>
       <c r="H36" s="41"/>
@@ -3278,7 +3328,7 @@
     </row>
     <row r="37" spans="1:20" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="79" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>1</v>
@@ -3296,13 +3346,13 @@
         <v>73</v>
       </c>
       <c r="G37" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="H37" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="H37" s="46" t="s">
-        <v>91</v>
-      </c>
       <c r="I37" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J37" s="46"/>
       <c r="M37" s="37"/>
@@ -3332,7 +3382,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I38" s="45"/>
       <c r="J38" s="16"/>
@@ -3357,14 +3407,14 @@
         <v>1</v>
       </c>
       <c r="H39" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="16"/>
     </row>
     <row r="40" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="80" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -3382,7 +3432,7 @@
         <v>4</v>
       </c>
       <c r="H40" s="42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I40" s="45"/>
       <c r="J40" s="16"/>
@@ -3398,7 +3448,7 @@
         <v>4</v>
       </c>
       <c r="H41" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I41" s="45"/>
       <c r="J41" s="44"/>
@@ -3429,7 +3479,7 @@
         <v>73</v>
       </c>
       <c r="P42" s="51" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
@@ -3442,7 +3492,7 @@
         <v>1</v>
       </c>
       <c r="N43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O43">
         <v>1</v>
@@ -3453,7 +3503,7 @@
     </row>
     <row r="44" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="81" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -3468,7 +3518,7 @@
         <v>2</v>
       </c>
       <c r="N44" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O44">
         <v>2</v>
@@ -3480,7 +3530,7 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="81" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>66</v>
@@ -3492,7 +3542,7 @@
         <v>3</v>
       </c>
       <c r="N45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O45">
         <v>3</v>
@@ -3504,13 +3554,13 @@
     </row>
     <row r="46" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="81" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D46" t="s">
         <v>74</v>
@@ -3519,16 +3569,16 @@
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M46" s="6">
         <v>4</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O46">
         <v>4</v>
@@ -3550,7 +3600,7 @@
         <v>5</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O47">
         <v>5</v>
@@ -3561,7 +3611,7 @@
     </row>
     <row r="48" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="81" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F48" s="5"/>
       <c r="K48" s="6"/>
@@ -3569,7 +3619,7 @@
         <v>6</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O48">
         <v>6</v>
@@ -3585,7 +3635,7 @@
         <v>7</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O49">
         <v>1</v>
@@ -3593,13 +3643,13 @@
     </row>
     <row r="50" spans="1:32" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="89" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F50" s="5"/>
       <c r="K50" s="6"/>
       <c r="L50" s="66"/>
       <c r="M50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:32" x14ac:dyDescent="0.3">
@@ -3623,24 +3673,34 @@
     </row>
     <row r="55" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="90" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C55" s="39"/>
       <c r="D55" s="63"/>
       <c r="E55" s="92" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F55" s="52"/>
       <c r="G55" s="52"/>
       <c r="H55" s="52"/>
       <c r="I55" s="52"/>
-      <c r="J55" s="92" t="s">
-        <v>228</v>
-      </c>
-      <c r="K55" s="52"/>
+      <c r="J55" s="95"/>
+      <c r="K55" s="99" t="s">
+        <v>227</v>
+      </c>
       <c r="L55" s="52"/>
       <c r="M55" s="52"/>
       <c r="N55" s="52"/>
+      <c r="O55" s="52"/>
+      <c r="U55"/>
+      <c r="V55" s="1"/>
+      <c r="X55"/>
+      <c r="Y55" s="1"/>
+      <c r="AA55"/>
+      <c r="AB55" s="5"/>
+      <c r="AC55" s="6"/>
+      <c r="AD55"/>
+      <c r="AE55" s="5"/>
     </row>
     <row r="56" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="59" t="s">
@@ -3650,52 +3710,67 @@
         <v>22</v>
       </c>
       <c r="D56" s="59" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E56" s="91" t="s">
         <v>1</v>
       </c>
       <c r="F56" s="91" t="s">
-        <v>75</v>
+        <v>285</v>
       </c>
       <c r="G56" s="91" t="s">
-        <v>90</v>
+        <v>284</v>
       </c>
       <c r="H56" s="91" t="s">
+        <v>89</v>
+      </c>
+      <c r="I56" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="I56" s="91" t="s">
+      <c r="J56" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="J56" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="K56" s="91" t="s">
+      <c r="K56" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="L56" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="L56" s="91" t="s">
-        <v>275</v>
-      </c>
       <c r="M56" s="91" t="s">
+        <v>274</v>
+      </c>
+      <c r="N56" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="N56" s="91" t="s">
-        <v>280</v>
-      </c>
+      <c r="O56" s="91" t="s">
+        <v>279</v>
+      </c>
+      <c r="P56" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="U56"/>
+      <c r="V56" s="1"/>
+      <c r="X56"/>
+      <c r="Y56" s="1"/>
+      <c r="AA56"/>
+      <c r="AB56" s="5"/>
+      <c r="AC56" s="6"/>
+      <c r="AD56"/>
+      <c r="AE56" s="5"/>
     </row>
     <row r="57" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B57" s="20">
         <v>1</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D57" s="64" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E57" s="6"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="6"/>
+      <c r="J57" s="97"/>
+      <c r="K57" s="101"/>
       <c r="L57" s="6"/>
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.3">
@@ -3703,15 +3778,15 @@
         <v>2</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D58" s="64" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E58"/>
       <c r="F58" s="6"/>
-      <c r="J58" s="5"/>
-      <c r="K58" s="6"/>
+      <c r="J58" s="97"/>
+      <c r="K58" s="101"/>
       <c r="L58" s="6"/>
     </row>
     <row r="59" spans="1:32" x14ac:dyDescent="0.3">
@@ -3719,15 +3794,15 @@
         <v>3</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D59" s="64" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
-      <c r="J59" s="5"/>
-      <c r="K59" s="6"/>
+      <c r="J59" s="97"/>
+      <c r="K59" s="101"/>
       <c r="L59" s="6"/>
     </row>
     <row r="60" spans="1:32" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -3736,7 +3811,8 @@
       <c r="D60" s="64"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
-      <c r="J60" s="5"/>
+      <c r="J60" s="97"/>
+      <c r="K60" s="102"/>
       <c r="L60" s="6"/>
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.3">
@@ -3745,7 +3821,8 @@
       <c r="D61" s="64"/>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
-      <c r="J61" s="5"/>
+      <c r="J61" s="97"/>
+      <c r="K61" s="102"/>
       <c r="L61" s="6"/>
       <c r="N61" s="6"/>
     </row>
@@ -3758,15 +3835,15 @@
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
-      <c r="J62" s="94"/>
-      <c r="K62" s="8"/>
+      <c r="J62" s="98"/>
+      <c r="K62" s="103"/>
       <c r="L62" s="8"/>
       <c r="M62" s="8"/>
       <c r="N62" s="8"/>
     </row>
     <row r="63" spans="1:32" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A63" s="93" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -3793,7 +3870,7 @@
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B64" s="60" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C64" s="60" t="s">
         <v>71</v>
@@ -3803,10 +3880,10 @@
       <c r="F64" s="60"/>
       <c r="G64" s="61"/>
       <c r="H64" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I64" s="88" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L64" s="6"/>
       <c r="N64" s="6"/>
@@ -3822,43 +3899,43 @@
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B65" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="C65" s="59" t="s">
+        <v>233</v>
+      </c>
+      <c r="D65" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="E65" s="59" t="s">
+        <v>280</v>
+      </c>
+      <c r="F65" s="59" t="s">
+        <v>239</v>
+      </c>
+      <c r="G65" s="87" t="s">
+        <v>255</v>
+      </c>
+      <c r="H65" s="62" t="s">
+        <v>235</v>
+      </c>
+      <c r="I65" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="C65" s="59" t="s">
+      <c r="J65" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="K65" s="62" t="s">
         <v>234</v>
       </c>
-      <c r="D65" s="59" t="s">
-        <v>232</v>
-      </c>
-      <c r="E65" s="59" t="s">
-        <v>281</v>
-      </c>
-      <c r="F65" s="59" t="s">
-        <v>240</v>
-      </c>
-      <c r="G65" s="87" t="s">
-        <v>256</v>
-      </c>
-      <c r="H65" s="62" t="s">
-        <v>236</v>
-      </c>
-      <c r="I65" s="62" t="s">
-        <v>237</v>
-      </c>
-      <c r="J65" s="62" t="s">
-        <v>238</v>
-      </c>
-      <c r="K65" s="62" t="s">
-        <v>235</v>
-      </c>
       <c r="L65" s="62" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M65" s="62" t="s">
+        <v>275</v>
+      </c>
+      <c r="N65" s="62" t="s">
         <v>276</v>
-      </c>
-      <c r="N65" s="62" t="s">
-        <v>277</v>
       </c>
       <c r="U65"/>
       <c r="W65" s="1"/>
@@ -3872,7 +3949,7 @@
     </row>
     <row r="66" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" s="84" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E66"/>
       <c r="F66" s="4"/>
@@ -3937,7 +4014,7 @@
     </row>
     <row r="68" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="84" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E68"/>
       <c r="F68" s="4"/>
@@ -3971,7 +4048,7 @@
     </row>
     <row r="69" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="84" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E69"/>
       <c r="F69" s="4"/>
@@ -4035,8 +4112,8 @@
       <c r="AE70" s="5"/>
     </row>
     <row r="71" spans="1:32" ht="72" x14ac:dyDescent="0.3">
-      <c r="A71" s="95" t="s">
-        <v>278</v>
+      <c r="A71" s="94" t="s">
+        <v>277</v>
       </c>
       <c r="E71"/>
       <c r="F71" s="4"/>
@@ -4092,13 +4169,13 @@
     <row r="74" spans="1:32" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="73"/>
       <c r="B74" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D74" s="86"/>
       <c r="E74" s="86"/>
       <c r="G74" s="67"/>
       <c r="H74" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I74" s="69"/>
       <c r="J74" s="69"/>
@@ -4112,22 +4189,22 @@
     </row>
     <row r="75" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A75" s="74" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B75" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="C75" s="59" t="s">
         <v>236</v>
       </c>
-      <c r="C75" s="59" t="s">
-        <v>237</v>
-      </c>
       <c r="D75" s="59" t="s">
+        <v>282</v>
+      </c>
+      <c r="E75" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="F75" s="59" t="s">
         <v>283</v>
-      </c>
-      <c r="E75" s="59" t="s">
-        <v>247</v>
-      </c>
-      <c r="F75" s="59" t="s">
-        <v>284</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" s="59" t="s">
@@ -4137,7 +4214,7 @@
         <v>22</v>
       </c>
       <c r="J75" s="59" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K75" s="59"/>
       <c r="L75" s="59"/>
@@ -4152,7 +4229,7 @@
         <v>1</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
@@ -4160,7 +4237,7 @@
     </row>
     <row r="77" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="74" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B77" s="13">
         <v>2</v>
@@ -4177,7 +4254,7 @@
     </row>
     <row r="78" spans="1:32" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A78" s="79" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B78" s="13">
         <v>3</v>
@@ -4220,7 +4297,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="74" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B81" s="13">
         <v>6</v>
@@ -4235,7 +4312,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="74" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B82" s="13">
         <v>7</v>
@@ -4248,7 +4325,7 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="74" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="1"/>
@@ -4257,7 +4334,7 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="74" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="1"/>
@@ -4266,7 +4343,7 @@
     </row>
     <row r="85" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A85" s="74" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F85" s="6"/>
       <c r="G85" s="1"/>
@@ -4275,10 +4352,10 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="74" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C86" s="13"/>
       <c r="F86" s="6"/>
@@ -4288,22 +4365,22 @@
     </row>
     <row r="87" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A87" s="74" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B87" s="59" t="s">
         <v>1</v>
       </c>
       <c r="C87" s="59" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D87" s="59" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E87" s="59"/>
       <c r="F87" s="59"/>
       <c r="G87" s="1"/>
       <c r="H87" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L87" s="6"/>
     </row>
@@ -4399,7 +4476,7 @@
     </row>
     <row r="98" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B98" s="48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
@@ -4424,13 +4501,13 @@
     </row>
     <row r="100" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B100" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C100" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="C100" s="40" t="s">
+      <c r="D100" s="40" t="s">
         <v>96</v>
-      </c>
-      <c r="D100" s="40" t="s">
-        <v>97</v>
       </c>
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
@@ -4444,13 +4521,13 @@
     </row>
     <row r="101" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B101" s="41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C101" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D101" s="41" t="s">
         <v>98</v>
-      </c>
-      <c r="D101" s="41" t="s">
-        <v>99</v>
       </c>
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
@@ -4464,13 +4541,13 @@
     </row>
     <row r="102" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B102" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C102" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="C102" s="41" t="s">
+      <c r="D102" s="41" t="s">
         <v>101</v>
-      </c>
-      <c r="D102" s="41" t="s">
-        <v>102</v>
       </c>
       <c r="F102" s="6"/>
       <c r="G102" s="6"/>
@@ -4487,10 +4564,10 @@
         <v>27</v>
       </c>
       <c r="C103" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D103" s="41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F103" s="6"/>
       <c r="G103" s="6"/>
@@ -4507,10 +4584,10 @@
         <v>2</v>
       </c>
       <c r="C104" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D104" s="41" t="s">
         <v>104</v>
-      </c>
-      <c r="D104" s="41" t="s">
-        <v>105</v>
       </c>
       <c r="F104" s="6"/>
       <c r="G104" s="6"/>
@@ -4524,13 +4601,13 @@
     </row>
     <row r="105" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B105" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C105" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C105" s="41" t="s">
+      <c r="D105" s="41" t="s">
         <v>107</v>
-      </c>
-      <c r="D105" s="41" t="s">
-        <v>108</v>
       </c>
       <c r="F105" s="6"/>
       <c r="G105" s="6"/>
@@ -4544,13 +4621,13 @@
     </row>
     <row r="106" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B106" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C106" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C106" s="41" t="s">
+      <c r="D106" s="41" t="s">
         <v>110</v>
-      </c>
-      <c r="D106" s="41" t="s">
-        <v>111</v>
       </c>
       <c r="F106" s="6"/>
       <c r="G106" s="6"/>
@@ -4564,13 +4641,13 @@
     </row>
     <row r="107" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B107" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="C107" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D107" s="41" t="s">
         <v>112</v>
-      </c>
-      <c r="C107" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="D107" s="41" t="s">
-        <v>113</v>
       </c>
       <c r="F107" s="6"/>
       <c r="G107" s="6"/>
@@ -4584,13 +4661,13 @@
     </row>
     <row r="108" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B108" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C108" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="C108" s="41" t="s">
+      <c r="D108" s="41" t="s">
         <v>115</v>
-      </c>
-      <c r="D108" s="41" t="s">
-        <v>116</v>
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
@@ -4615,7 +4692,7 @@
     </row>
     <row r="110" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B110" s="48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F110" s="6"/>
       <c r="G110" s="6"/>
@@ -4640,13 +4717,13 @@
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B112" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C112" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="C112" s="40" t="s">
+      <c r="D112" s="40" t="s">
         <v>96</v>
-      </c>
-      <c r="D112" s="40" t="s">
-        <v>97</v>
       </c>
       <c r="F112" s="6"/>
       <c r="G112" s="6"/>
@@ -4663,10 +4740,10 @@
         <v>64</v>
       </c>
       <c r="C113" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D113" s="41" t="s">
         <v>98</v>
-      </c>
-      <c r="D113" s="41" t="s">
-        <v>99</v>
       </c>
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
@@ -4683,10 +4760,10 @@
         <v>0</v>
       </c>
       <c r="C114" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D114" s="41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F114" s="6"/>
       <c r="G114" s="6"/>
@@ -4700,13 +4777,13 @@
     </row>
     <row r="115" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B115" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C115" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D115" s="41" t="s">
         <v>119</v>
-      </c>
-      <c r="C115" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D115" s="41" t="s">
-        <v>120</v>
       </c>
       <c r="F115" s="6"/>
       <c r="G115" s="6"/>
@@ -4720,13 +4797,13 @@
     </row>
     <row r="116" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B116" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C116" s="41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D116" s="41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F116" s="6"/>
       <c r="G116" s="6"/>
@@ -4740,13 +4817,13 @@
     </row>
     <row r="117" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B117" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C117" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D117" s="41" t="s">
         <v>122</v>
-      </c>
-      <c r="C117" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="D117" s="41" t="s">
-        <v>123</v>
       </c>
       <c r="F117" s="6"/>
       <c r="G117" s="6"/>
@@ -4760,13 +4837,13 @@
     </row>
     <row r="118" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B118" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C118" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D118" s="41" t="s">
         <v>124</v>
-      </c>
-      <c r="C118" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="D118" s="41" t="s">
-        <v>125</v>
       </c>
       <c r="F118" s="6"/>
       <c r="G118" s="6"/>
@@ -4780,13 +4857,13 @@
     </row>
     <row r="119" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B119" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C119" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D119" s="41" t="s">
         <v>126</v>
-      </c>
-      <c r="C119" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="D119" s="41" t="s">
-        <v>127</v>
       </c>
       <c r="F119" s="6"/>
       <c r="G119" s="6"/>
@@ -4800,13 +4877,13 @@
     </row>
     <row r="120" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B120" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C120" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D120" s="41" t="s">
         <v>128</v>
-      </c>
-      <c r="C120" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="D120" s="41" t="s">
-        <v>129</v>
       </c>
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
@@ -4820,13 +4897,13 @@
     </row>
     <row r="121" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B121" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C121" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C121" s="41" t="s">
-        <v>110</v>
-      </c>
       <c r="D121" s="41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F121" s="6"/>
       <c r="G121" s="6"/>
@@ -4840,13 +4917,13 @@
     </row>
     <row r="122" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B122" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C122" s="41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D122" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F122" s="6"/>
       <c r="G122" s="6"/>
@@ -4871,7 +4948,7 @@
     </row>
     <row r="124" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B124" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F124" s="6"/>
       <c r="G124" s="6"/>
@@ -4896,13 +4973,13 @@
     </row>
     <row r="126" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B126" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C126" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="C126" s="40" t="s">
+      <c r="D126" s="40" t="s">
         <v>96</v>
-      </c>
-      <c r="D126" s="40" t="s">
-        <v>97</v>
       </c>
       <c r="F126" s="6"/>
       <c r="G126" s="6"/>
@@ -4919,10 +4996,10 @@
         <v>73</v>
       </c>
       <c r="C127" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D127" s="41" t="s">
         <v>98</v>
-      </c>
-      <c r="D127" s="41" t="s">
-        <v>99</v>
       </c>
       <c r="F127" s="6"/>
       <c r="G127" s="6"/>
@@ -4936,13 +5013,13 @@
     </row>
     <row r="128" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B128" s="41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C128" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D128" s="41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F128" s="6"/>
       <c r="G128" s="6"/>
@@ -4956,13 +5033,13 @@
     </row>
     <row r="129" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B129" s="41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C129" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D129" s="41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F129" s="6"/>
       <c r="G129" s="6"/>
@@ -4976,13 +5053,13 @@
     </row>
     <row r="130" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B130" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C130" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D130" s="41" t="s">
         <v>135</v>
-      </c>
-      <c r="C130" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="D130" s="41" t="s">
-        <v>136</v>
       </c>
       <c r="F130" s="6"/>
       <c r="G130" s="6"/>
@@ -4996,13 +5073,13 @@
     </row>
     <row r="131" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B131" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C131" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D131" s="41" t="s">
         <v>137</v>
-      </c>
-      <c r="C131" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="D131" s="41" t="s">
-        <v>138</v>
       </c>
       <c r="F131" s="6"/>
       <c r="G131" s="6"/>
@@ -5016,13 +5093,13 @@
     </row>
     <row r="132" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B132" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C132" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C132" s="41" t="s">
-        <v>110</v>
-      </c>
       <c r="D132" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F132" s="6"/>
       <c r="G132" s="6"/>
@@ -5036,13 +5113,13 @@
     </row>
     <row r="133" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B133" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C133" s="41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D133" s="41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F133" s="6"/>
       <c r="G133" s="6"/>
@@ -5067,7 +5144,7 @@
     </row>
     <row r="135" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B135" s="48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F135" s="6"/>
       <c r="G135" s="6"/>
@@ -5092,13 +5169,13 @@
     </row>
     <row r="137" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B137" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C137" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="C137" s="40" t="s">
+      <c r="D137" s="40" t="s">
         <v>96</v>
-      </c>
-      <c r="D137" s="40" t="s">
-        <v>97</v>
       </c>
       <c r="F137" s="6"/>
       <c r="G137" s="6"/>
@@ -5112,13 +5189,13 @@
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B138" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C138" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D138" s="41" t="s">
         <v>98</v>
-      </c>
-      <c r="D138" s="41" t="s">
-        <v>99</v>
       </c>
       <c r="F138" s="6"/>
       <c r="G138" s="6"/>
@@ -5135,10 +5212,10 @@
         <v>73</v>
       </c>
       <c r="C139" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D139" s="41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F139" s="6"/>
       <c r="G139" s="6"/>
@@ -5155,10 +5232,10 @@
         <v>64</v>
       </c>
       <c r="C140" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D140" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F140" s="6"/>
       <c r="G140" s="6"/>
@@ -5175,10 +5252,10 @@
         <v>3</v>
       </c>
       <c r="C141" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D141" s="41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F141" s="6"/>
       <c r="G141" s="6"/>
@@ -5192,13 +5269,13 @@
     </row>
     <row r="142" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B142" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C142" s="41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D142" s="41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F142" s="6"/>
       <c r="G142" s="6"/>
@@ -5212,13 +5289,13 @@
     </row>
     <row r="143" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B143" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C143" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C143" s="41" t="s">
-        <v>110</v>
-      </c>
       <c r="D143" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F143" s="6"/>
       <c r="G143" s="6"/>
@@ -5232,13 +5309,13 @@
     </row>
     <row r="144" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B144" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C144" s="41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D144" s="41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F144" s="6"/>
       <c r="G144" s="6"/>
@@ -5263,7 +5340,7 @@
     </row>
     <row r="146" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B146" s="48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F146" s="6"/>
       <c r="G146" s="6"/>
@@ -5288,13 +5365,13 @@
     </row>
     <row r="148" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B148" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C148" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="C148" s="40" t="s">
+      <c r="D148" s="40" t="s">
         <v>96</v>
-      </c>
-      <c r="D148" s="40" t="s">
-        <v>97</v>
       </c>
       <c r="F148" s="6"/>
       <c r="G148" s="6"/>
@@ -5308,13 +5385,13 @@
     </row>
     <row r="149" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B149" s="41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C149" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D149" s="41" t="s">
         <v>98</v>
-      </c>
-      <c r="D149" s="41" t="s">
-        <v>99</v>
       </c>
       <c r="F149" s="6"/>
       <c r="G149" s="6"/>
@@ -5328,13 +5405,13 @@
     </row>
     <row r="150" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B150" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="C150" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D150" s="41" t="s">
         <v>148</v>
-      </c>
-      <c r="C150" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D150" s="41" t="s">
-        <v>149</v>
       </c>
       <c r="F150" s="6"/>
       <c r="G150" s="6"/>
@@ -5348,13 +5425,13 @@
     </row>
     <row r="151" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B151" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="C151" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D151" s="41" t="s">
         <v>150</v>
-      </c>
-      <c r="C151" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D151" s="41" t="s">
-        <v>151</v>
       </c>
       <c r="F151" s="6"/>
       <c r="G151" s="6"/>
@@ -5368,13 +5445,13 @@
     </row>
     <row r="152" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B152" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="C152" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="C152" s="41" t="s">
+      <c r="D152" s="41" t="s">
         <v>153</v>
-      </c>
-      <c r="D152" s="41" t="s">
-        <v>154</v>
       </c>
       <c r="F152" s="6"/>
       <c r="G152" s="6"/>
@@ -5388,13 +5465,13 @@
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B153" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="C153" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D153" s="41" t="s">
         <v>155</v>
-      </c>
-      <c r="C153" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D153" s="41" t="s">
-        <v>156</v>
       </c>
       <c r="F153" s="6"/>
       <c r="G153" s="6"/>
@@ -5408,13 +5485,13 @@
     </row>
     <row r="154" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B154" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="C154" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D154" s="41" t="s">
         <v>157</v>
-      </c>
-      <c r="C154" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="D154" s="41" t="s">
-        <v>158</v>
       </c>
       <c r="F154" s="6"/>
       <c r="G154" s="6"/>
@@ -5428,13 +5505,13 @@
     </row>
     <row r="155" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B155" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C155" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C155" s="41" t="s">
-        <v>110</v>
-      </c>
       <c r="D155" s="41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F155" s="6"/>
       <c r="G155" s="6"/>
@@ -5448,13 +5525,13 @@
     </row>
     <row r="156" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B156" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C156" s="41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D156" s="41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F156" s="6"/>
       <c r="G156" s="6"/>
@@ -5479,7 +5556,7 @@
     </row>
     <row r="158" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B158" s="48" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F158" s="6"/>
       <c r="G158" s="6"/>
@@ -5505,7 +5582,7 @@
     </row>
     <row r="160" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B160" s="49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F160" s="6"/>
       <c r="G160" s="6"/>
@@ -5519,7 +5596,7 @@
     </row>
     <row r="161" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B161" s="49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F161" s="6"/>
       <c r="G161" s="6"/>
@@ -5533,7 +5610,7 @@
     </row>
     <row r="162" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B162" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F162" s="6"/>
       <c r="G162" s="6"/>
@@ -5547,7 +5624,7 @@
     </row>
     <row r="163" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B163" s="49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F163" s="6"/>
       <c r="G163" s="6"/>
@@ -5561,7 +5638,7 @@
     </row>
     <row r="164" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B164" s="49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F164" s="6"/>
       <c r="G164" s="6"/>
@@ -5575,7 +5652,7 @@
     </row>
     <row r="165" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B165" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F165" s="6"/>
       <c r="G165" s="6"/>
@@ -5589,7 +5666,7 @@
     </row>
     <row r="166" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B166" s="49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F166" s="6"/>
       <c r="G166" s="6"/>
@@ -5603,7 +5680,7 @@
     </row>
     <row r="167" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B167" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F167" s="6"/>
       <c r="G167" s="6"/>
@@ -5617,7 +5694,7 @@
     </row>
     <row r="168" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B168" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F168" s="6"/>
       <c r="G168" s="6"/>
@@ -5631,7 +5708,7 @@
     </row>
     <row r="169" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B169" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F169" s="6"/>
       <c r="G169" s="6"/>
@@ -5645,7 +5722,7 @@
     </row>
     <row r="170" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B170" s="49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F170" s="6"/>
       <c r="G170" s="6"/>
@@ -5659,7 +5736,7 @@
     </row>
     <row r="171" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B171" s="49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F171" s="6"/>
       <c r="G171" s="6"/>
@@ -5685,7 +5762,7 @@
     </row>
     <row r="173" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B173" s="49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F173" s="6"/>
       <c r="G173" s="6"/>
@@ -5699,7 +5776,7 @@
     </row>
     <row r="174" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B174" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F174" s="6"/>
       <c r="G174" s="6"/>
@@ -5713,7 +5790,7 @@
     </row>
     <row r="175" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B175" s="49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F175" s="6"/>
       <c r="G175" s="6"/>
@@ -5727,7 +5804,7 @@
     </row>
     <row r="176" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B176" s="49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F176" s="6"/>
       <c r="G176" s="6"/>
@@ -5741,7 +5818,7 @@
     </row>
     <row r="177" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B177" s="49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F177" s="6"/>
       <c r="G177" s="6"/>
@@ -5755,7 +5832,7 @@
     </row>
     <row r="178" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B178" s="49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F178" s="6"/>
       <c r="G178" s="6"/>
@@ -5769,7 +5846,7 @@
     </row>
     <row r="179" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B179" s="49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F179" s="6"/>
       <c r="G179" s="6"/>
@@ -5783,7 +5860,7 @@
     </row>
     <row r="180" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B180" s="49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F180" s="6"/>
       <c r="G180" s="6"/>
@@ -5797,7 +5874,7 @@
     </row>
     <row r="181" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B181" s="49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F181" s="6"/>
       <c r="G181" s="6"/>
@@ -5811,7 +5888,7 @@
     </row>
     <row r="182" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B182" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F182" s="6"/>
       <c r="G182" s="6"/>
@@ -5825,7 +5902,7 @@
     </row>
     <row r="183" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B183" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F183" s="6"/>
       <c r="G183" s="6"/>
@@ -5839,7 +5916,7 @@
     </row>
     <row r="184" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B184" s="49" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F184" s="6"/>
       <c r="G184" s="6"/>
@@ -5853,7 +5930,7 @@
     </row>
     <row r="185" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B185" s="49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F185" s="6"/>
       <c r="G185" s="6"/>
@@ -5879,7 +5956,7 @@
     </row>
     <row r="187" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B187" s="49" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F187" s="6"/>
       <c r="G187" s="6"/>
@@ -5893,7 +5970,7 @@
     </row>
     <row r="188" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B188" s="49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F188" s="6"/>
       <c r="G188" s="6"/>
@@ -5907,7 +5984,7 @@
     </row>
     <row r="189" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B189" s="49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F189" s="6"/>
       <c r="G189" s="6"/>
@@ -5921,7 +5998,7 @@
     </row>
     <row r="190" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B190" s="49" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F190" s="6"/>
       <c r="G190" s="6"/>
@@ -5935,7 +6012,7 @@
     </row>
     <row r="191" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B191" s="49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F191" s="6"/>
       <c r="G191" s="6"/>
@@ -5949,7 +6026,7 @@
     </row>
     <row r="192" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B192" s="49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F192" s="6"/>
       <c r="G192" s="6"/>
@@ -5963,7 +6040,7 @@
     </row>
     <row r="193" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B193" s="49" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F193" s="6"/>
       <c r="G193" s="6"/>
@@ -5977,7 +6054,7 @@
     </row>
     <row r="194" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B194" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F194" s="6"/>
       <c r="G194" s="6"/>
@@ -5991,7 +6068,7 @@
     </row>
     <row r="195" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B195" s="49" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F195" s="6"/>
       <c r="G195" s="6"/>
@@ -6005,7 +6082,7 @@
     </row>
     <row r="196" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B196" s="49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F196" s="6"/>
       <c r="G196" s="6"/>
@@ -6031,7 +6108,7 @@
     </row>
     <row r="198" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B198" s="49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F198" s="6"/>
       <c r="G198" s="6"/>
@@ -6045,7 +6122,7 @@
     </row>
     <row r="199" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B199" s="49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F199" s="6"/>
       <c r="G199" s="6"/>
@@ -6059,7 +6136,7 @@
     </row>
     <row r="200" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B200" s="49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F200" s="6"/>
       <c r="G200" s="6"/>
@@ -6073,7 +6150,7 @@
     </row>
     <row r="201" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B201" s="49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F201" s="6"/>
       <c r="G201" s="6"/>
@@ -6087,7 +6164,7 @@
     </row>
     <row r="202" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B202" s="49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F202" s="6"/>
       <c r="G202" s="6"/>
@@ -6101,27 +6178,27 @@
     </row>
     <row r="203" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B203" s="49" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="204" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B204" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="205" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B205" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="206" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B206" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="207" spans="2:14" ht="15" x14ac:dyDescent="0.3">
       <c r="B207" s="49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="208" spans="2:14" x14ac:dyDescent="0.3">
@@ -6129,57 +6206,57 @@
     </row>
     <row r="209" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B209" s="49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="210" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B210" s="49" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="211" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B211" s="49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="212" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B212" s="49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="213" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B213" s="49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="214" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B214" s="49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="215" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B215" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="216" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B216" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="217" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B217" s="49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="218" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B218" s="49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="219" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B219" s="49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WENT MOST OF THE WAY WITH THE DATA MODELING
</commit_message>
<xml_diff>
--- a/DATA_MODELING AND WORKING.xlsx
+++ b/DATA_MODELING AND WORKING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktemi\code\dabo_bet\dabo_bet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AB8D67-924D-4F62-B7AC-5C05B47D160F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA42C1B6-E7DE-408A-B6DD-9D15DFF907B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{194E8500-D8EB-4916-9E2D-0F0C34382F12}"/>
   </bookViews>
@@ -1931,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67ECA014-9817-46D2-9F0E-849D0BDD3F91}">
   <dimension ref="A1:AF219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P56" sqref="P56"/>
+    <sheetView tabSelected="1" topLeftCell="G63" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>